<commit_message>
se agrega esbeltos, guia de uso y se amplia base de datos CIRSOC (en progreso)
</commit_message>
<xml_diff>
--- a/database/cirsoc-shapes-database.xlsx
+++ b/database/cirsoc-shapes-database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fce452423585d2c6/01.PERSONAL/Data Science/Proyectos/Estructuras metálicas/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perfiles-verificacion\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{CE1130F7-5636-42FF-AC96-9EEC076F729A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C51F624-1F15-49EA-8D7E-F1D56400538F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D99D37-35CF-4EAA-8F87-CE5A518E0741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C08AFA35-A25A-4CF1-A643-3A8FDC4FDF0E}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLA" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="751">
   <si>
     <t>Tipo</t>
   </si>
@@ -2396,6 +2396,624 @@
       </rPr>
       <t>1</t>
     </r>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>[mm]</t>
+  </si>
+  <si>
+    <t>[m2/m]</t>
+  </si>
+  <si>
+    <t>[cm222]</t>
+  </si>
+  <si>
+    <t>[Kg/m]</t>
+  </si>
+  <si>
+    <t>[cm4]</t>
+  </si>
+  <si>
+    <t>[cm3]</t>
+  </si>
+  <si>
+    <t>[cm]</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>22.22</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>1.04</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>1.31</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>1.39</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
+    <t>1.47</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>25.4</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>1.80</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>2.39</t>
+  </si>
+  <si>
+    <t>1.88</t>
+  </si>
+  <si>
+    <t>1.09</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>2.08</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>1.52</t>
+  </si>
+  <si>
+    <t>1.73</t>
+  </si>
+  <si>
+    <t>1.46</t>
+  </si>
+  <si>
+    <t>3.45</t>
+  </si>
+  <si>
+    <t>2.18</t>
+  </si>
+  <si>
+    <t>1.87</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>1.77</t>
+  </si>
+  <si>
+    <t>4.15</t>
+  </si>
+  <si>
+    <t>2.62</t>
+  </si>
+  <si>
+    <t>2.30</t>
+  </si>
+  <si>
+    <t>2.47</t>
+  </si>
+  <si>
+    <t>1.56</t>
+  </si>
+  <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>4.95</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>31.75</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>2.87</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>5.92</t>
+  </si>
+  <si>
+    <t>3.73</t>
+  </si>
+  <si>
+    <t>1.82</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>3.64</t>
+  </si>
+  <si>
+    <t>1.96</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>2.46</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>4.92</t>
+  </si>
+  <si>
+    <t>2.66</t>
+  </si>
+  <si>
+    <t>1.44</t>
+  </si>
+  <si>
+    <t>3.06</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>6.12</t>
+  </si>
+  <si>
+    <t>3.35</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>1.78</t>
+  </si>
+  <si>
+    <t>3.71</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>2.61</t>
+  </si>
+  <si>
+    <t>7.41</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>2.80</t>
+  </si>
+  <si>
+    <t>2.19</t>
+  </si>
+  <si>
+    <t>4.45</t>
+  </si>
+  <si>
+    <t>2.34</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>3.17</t>
+  </si>
+  <si>
+    <t>8.90</t>
+  </si>
+  <si>
+    <t>4.67</t>
+  </si>
+  <si>
+    <t>38.10</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>5.39</t>
+  </si>
+  <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>3.91</t>
+  </si>
+  <si>
+    <t>10.77</t>
+  </si>
+  <si>
+    <t>5.66</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>2.92</t>
+  </si>
+  <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>1.71</t>
+  </si>
+  <si>
+    <t>5.84</t>
+  </si>
+  <si>
+    <t>2.68</t>
+  </si>
+  <si>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>3.96</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>2.33</t>
+  </si>
+  <si>
+    <t>7.92</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>1.69</t>
+  </si>
+  <si>
+    <t>2.23</t>
+  </si>
+  <si>
+    <t>2.94</t>
+  </si>
+  <si>
+    <t>9.90</t>
+  </si>
+  <si>
+    <t>4.61</t>
+  </si>
+  <si>
+    <t>2.67</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>6.02</t>
+  </si>
+  <si>
+    <t>2.71</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>3.61</t>
+  </si>
+  <si>
+    <t>12.04</t>
+  </si>
+  <si>
+    <t>3.29</t>
+  </si>
+  <si>
+    <t>2.59</t>
+  </si>
+  <si>
+    <t>7.27</t>
+  </si>
+  <si>
+    <t>3.27</t>
+  </si>
+  <si>
+    <t>1.49</t>
+  </si>
+  <si>
+    <t>4.41</t>
+  </si>
+  <si>
+    <t>14.55</t>
+  </si>
+  <si>
+    <t>6.55</t>
+  </si>
+  <si>
+    <t>44.45</t>
+  </si>
+  <si>
+    <t>3.26</t>
+  </si>
+  <si>
+    <t>8.87</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>5.46</t>
+  </si>
+  <si>
+    <t>17.75</t>
+  </si>
+  <si>
+    <t>7.98</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>T 3/4 x 3/4 x 1/8</t>
+  </si>
+  <si>
+    <t>T 7/8 x 7/8 x 1/8</t>
+  </si>
+  <si>
+    <t>T 1 x 1 x 1/8</t>
+  </si>
+  <si>
+    <t>T 1 x 1 x 3/16</t>
+  </si>
+  <si>
+    <t>T 1 1/8 x 1 1/8 x 1/8</t>
+  </si>
+  <si>
+    <t>T 1 1/4 x 1 1/4 x 1/8</t>
+  </si>
+  <si>
+    <t>T 1 1/4 x 1 1/4 x 3/16</t>
+  </si>
+  <si>
+    <t>T 1 1/2 x 1 1/2 x 1/8</t>
+  </si>
+  <si>
+    <t>T 1 1/2 x 1 1/2 x 3/16</t>
+  </si>
+  <si>
+    <t>T 1 1/2 x 1 1/2 x 1/4</t>
+  </si>
+  <si>
+    <t>T 1 3/4 x 1 3/4 x 3/16</t>
+  </si>
+  <si>
+    <t>T 2 x 2 x 3/16</t>
+  </si>
+  <si>
+    <t>T 2 x 2 x 1/4</t>
+  </si>
+  <si>
+    <t>d/tw</t>
+  </si>
+  <si>
+    <t>dx</t>
   </si>
 </sst>
 </file>
@@ -2577,7 +3195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2651,6 +3269,25 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2686,10 +3323,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2989,24 +3622,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54AC280-589B-4A0A-9E63-8D2C52B28E53}">
-  <dimension ref="A1:BD515"/>
+  <dimension ref="A1:BF605"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AB293" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C548" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="J577" sqref="J577"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.5703125" customWidth="1"/>
     <col min="30" max="30" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3175,8 +3809,14 @@
       <c r="BD1" s="3" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="BE1" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
@@ -3279,7 +3919,7 @@
       <c r="AL2" s="9"/>
       <c r="AM2" s="19"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>31</v>
       </c>
@@ -3382,7 +4022,7 @@
       <c r="AL3" s="9"/>
       <c r="AM3" s="19"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
@@ -3485,7 +4125,7 @@
       <c r="AL4" s="9"/>
       <c r="AM4" s="19"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
@@ -3588,7 +4228,7 @@
       <c r="AL5" s="9"/>
       <c r="AM5" s="19"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>31</v>
       </c>
@@ -3691,7 +4331,7 @@
       <c r="AL6" s="9"/>
       <c r="AM6" s="19"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
@@ -3794,7 +4434,7 @@
       <c r="AL7" s="9"/>
       <c r="AM7" s="19"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>31</v>
       </c>
@@ -3897,7 +4537,7 @@
       <c r="AL8" s="9"/>
       <c r="AM8" s="19"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
@@ -4000,7 +4640,7 @@
       <c r="AL9" s="9"/>
       <c r="AM9" s="19"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>31</v>
       </c>
@@ -4103,7 +4743,7 @@
       <c r="AL10" s="9"/>
       <c r="AM10" s="19"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
@@ -4206,7 +4846,7 @@
       <c r="AL11" s="9"/>
       <c r="AM11" s="19"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>31</v>
       </c>
@@ -4309,7 +4949,7 @@
       <c r="AL12" s="9"/>
       <c r="AM12" s="19"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
@@ -4412,7 +5052,7 @@
       <c r="AL13" s="9"/>
       <c r="AM13" s="19"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
@@ -4515,7 +5155,7 @@
       <c r="AL14" s="9"/>
       <c r="AM14" s="19"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>31</v>
       </c>
@@ -4618,7 +5258,7 @@
       <c r="AL15" s="9"/>
       <c r="AM15" s="19"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
@@ -51643,7 +52283,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="513" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A513" s="21" t="s">
         <v>449</v>
       </c>
@@ -51714,7 +52354,7 @@
         <v>5.96</v>
       </c>
     </row>
-    <row r="514" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A514" s="21" t="s">
         <v>449</v>
       </c>
@@ -51785,7 +52425,7 @@
         <v>5.93</v>
       </c>
     </row>
-    <row r="515" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A515" s="21" t="s">
         <v>449</v>
       </c>
@@ -51854,6 +52494,2482 @@
       </c>
       <c r="BD515" s="23">
         <v>5.91</v>
+      </c>
+    </row>
+    <row r="516" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A516" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B516" s="26" t="s">
+        <v>736</v>
+      </c>
+      <c r="C516" s="27">
+        <v>19</v>
+      </c>
+      <c r="D516" s="27">
+        <v>19</v>
+      </c>
+      <c r="E516" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I516" s="27">
+        <v>2.97</v>
+      </c>
+      <c r="K516" s="29">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="L516" s="29">
+        <v>0.89</v>
+      </c>
+      <c r="M516" s="31">
+        <v>0.33</v>
+      </c>
+      <c r="N516" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="O516" s="31">
+        <v>0.54</v>
+      </c>
+      <c r="P516" s="31">
+        <v>0.26</v>
+      </c>
+      <c r="Q516" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="R516" s="31">
+        <v>0.18</v>
+      </c>
+      <c r="S516" s="31">
+        <v>0.19</v>
+      </c>
+      <c r="T516" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="U516" s="31">
+        <v>0.16</v>
+      </c>
+      <c r="V516" s="31">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="W516" s="31">
+        <v>0.31</v>
+      </c>
+      <c r="AC516" s="31">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AD516" s="31">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="BE516" s="28">
+        <v>5.94</v>
+      </c>
+      <c r="BF516" s="30">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="517" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A517" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B517" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="C517" s="27">
+        <v>22</v>
+      </c>
+      <c r="D517" s="27">
+        <v>22</v>
+      </c>
+      <c r="E517" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I517" s="27">
+        <v>3.44</v>
+      </c>
+      <c r="K517" s="29">
+        <v>1.33</v>
+      </c>
+      <c r="L517" s="29">
+        <v>1.04</v>
+      </c>
+      <c r="M517" s="31">
+        <v>0.53</v>
+      </c>
+      <c r="N517" s="31">
+        <v>0.34</v>
+      </c>
+      <c r="O517" s="31">
+        <v>0.63</v>
+      </c>
+      <c r="P517" s="31">
+        <v>0.36</v>
+      </c>
+      <c r="Q517" s="31">
+        <v>0.67</v>
+      </c>
+      <c r="R517" s="31">
+        <v>0.27</v>
+      </c>
+      <c r="S517" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="T517" s="31">
+        <v>0.45</v>
+      </c>
+      <c r="U517" s="31">
+        <v>0.21</v>
+      </c>
+      <c r="V517" s="31">
+        <v>0.38</v>
+      </c>
+      <c r="W517" s="31">
+        <v>0.42</v>
+      </c>
+      <c r="AC517" s="31">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AD517" s="31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="BE517" s="28">
+        <v>6.88</v>
+      </c>
+      <c r="BF517" s="30">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="518" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A518" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B518" s="26" t="s">
+        <v>738</v>
+      </c>
+      <c r="C518" s="27">
+        <v>25</v>
+      </c>
+      <c r="D518" s="27">
+        <v>25</v>
+      </c>
+      <c r="E518" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I518" s="27">
+        <v>3.91</v>
+      </c>
+      <c r="K518" s="29">
+        <v>1.52</v>
+      </c>
+      <c r="L518" s="29">
+        <v>1.19</v>
+      </c>
+      <c r="M518" s="31">
+        <v>0.79</v>
+      </c>
+      <c r="N518" s="31">
+        <v>0.44</v>
+      </c>
+      <c r="O518" s="31">
+        <v>0.72</v>
+      </c>
+      <c r="P518" s="31">
+        <v>0.46</v>
+      </c>
+      <c r="Q518" s="31">
+        <v>0.89</v>
+      </c>
+      <c r="R518" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="S518" s="31">
+        <v>0.32</v>
+      </c>
+      <c r="T518" s="31">
+        <v>0.51</v>
+      </c>
+      <c r="U518" s="31">
+        <v>0.27</v>
+      </c>
+      <c r="V518" s="31">
+        <v>0.48</v>
+      </c>
+      <c r="W518" s="31">
+        <v>0.53</v>
+      </c>
+      <c r="AC518" s="31">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="AD518" s="31">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="BE518" s="28">
+        <v>7.81</v>
+      </c>
+      <c r="BF518" s="30">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="519" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A519" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B519" s="26" t="s">
+        <v>739</v>
+      </c>
+      <c r="C519" s="27">
+        <v>25</v>
+      </c>
+      <c r="D519" s="27">
+        <v>25</v>
+      </c>
+      <c r="E519" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="I519" s="27">
+        <v>2.6</v>
+      </c>
+      <c r="K519" s="29">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="L519" s="29">
+        <v>1.74</v>
+      </c>
+      <c r="M519" s="31">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="N519" s="31">
+        <v>0.65</v>
+      </c>
+      <c r="O519" s="31">
+        <v>0.71</v>
+      </c>
+      <c r="P519" s="31">
+        <v>0.67</v>
+      </c>
+      <c r="Q519" s="31">
+        <v>1.22</v>
+      </c>
+      <c r="R519" s="31">
+        <v>0.61</v>
+      </c>
+      <c r="S519" s="31">
+        <v>0.49</v>
+      </c>
+      <c r="T519" s="31">
+        <v>0.52</v>
+      </c>
+      <c r="U519" s="31">
+        <v>0.42</v>
+      </c>
+      <c r="V519" s="31">
+        <v>0.74</v>
+      </c>
+      <c r="W519" s="31">
+        <v>0.83</v>
+      </c>
+      <c r="AC519" s="31">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AD519" s="31">
+        <v>0.06</v>
+      </c>
+      <c r="BE519" s="28">
+        <v>5.21</v>
+      </c>
+      <c r="BF519" s="30">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="520" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A520" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B520" s="26" t="s">
+        <v>740</v>
+      </c>
+      <c r="C520" s="27">
+        <v>29</v>
+      </c>
+      <c r="D520" s="27">
+        <v>29</v>
+      </c>
+      <c r="E520" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I520" s="27">
+        <v>4.53</v>
+      </c>
+      <c r="K520" s="29">
+        <v>1.77</v>
+      </c>
+      <c r="L520" s="29">
+        <v>1.39</v>
+      </c>
+      <c r="M520" s="31">
+        <v>1.25</v>
+      </c>
+      <c r="N520" s="31">
+        <v>0.59</v>
+      </c>
+      <c r="O520" s="31">
+        <v>0.84</v>
+      </c>
+      <c r="P520" s="31">
+        <v>0.63</v>
+      </c>
+      <c r="Q520" s="31">
+        <v>1.22</v>
+      </c>
+      <c r="R520" s="31">
+        <v>0.62</v>
+      </c>
+      <c r="S520" s="31">
+        <v>0.43</v>
+      </c>
+      <c r="T520" s="31">
+        <v>0.59</v>
+      </c>
+      <c r="U520" s="31">
+        <v>0.35</v>
+      </c>
+      <c r="V520" s="31">
+        <v>0.65</v>
+      </c>
+      <c r="W520" s="31">
+        <v>0.71</v>
+      </c>
+      <c r="AC520" s="31">
+        <v>0.06</v>
+      </c>
+      <c r="AD520" s="31">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="BE520" s="28">
+        <v>9.06</v>
+      </c>
+      <c r="BF520" s="30">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="521" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A521" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B521" s="26" t="s">
+        <v>741</v>
+      </c>
+      <c r="C521" s="27">
+        <v>32</v>
+      </c>
+      <c r="D521" s="27">
+        <v>32</v>
+      </c>
+      <c r="E521" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I521" s="27">
+        <v>5</v>
+      </c>
+      <c r="K521" s="29">
+        <v>1.96</v>
+      </c>
+      <c r="L521" s="29">
+        <v>1.54</v>
+      </c>
+      <c r="M521" s="31">
+        <v>1.69</v>
+      </c>
+      <c r="N521" s="31">
+        <v>0.72</v>
+      </c>
+      <c r="O521" s="31">
+        <v>0.93</v>
+      </c>
+      <c r="P521" s="31">
+        <v>0.77</v>
+      </c>
+      <c r="Q521" s="31">
+        <v>1.48</v>
+      </c>
+      <c r="R521" s="31">
+        <v>0.83</v>
+      </c>
+      <c r="S521" s="31">
+        <v>0.52</v>
+      </c>
+      <c r="T521" s="31">
+        <v>0.65</v>
+      </c>
+      <c r="U521" s="31">
+        <v>0.43</v>
+      </c>
+      <c r="V521" s="31">
+        <v>0.78</v>
+      </c>
+      <c r="W521" s="31">
+        <v>0.86</v>
+      </c>
+      <c r="AC521" s="31">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AD521" s="31">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="BE521" s="28">
+        <v>10</v>
+      </c>
+      <c r="BF521" s="30">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="522" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A522" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B522" s="26" t="s">
+        <v>742</v>
+      </c>
+      <c r="C522" s="27">
+        <v>32</v>
+      </c>
+      <c r="D522" s="27">
+        <v>32</v>
+      </c>
+      <c r="E522" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="I522" s="27">
+        <v>3.33</v>
+      </c>
+      <c r="K522" s="29">
+        <v>2.89</v>
+      </c>
+      <c r="L522" s="29">
+        <v>2.27</v>
+      </c>
+      <c r="M522" s="31">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N522" s="31">
+        <v>1.08</v>
+      </c>
+      <c r="O522" s="31">
+        <v>0.92</v>
+      </c>
+      <c r="P522" s="31">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Q522" s="31">
+        <v>2.11</v>
+      </c>
+      <c r="R522" s="31">
+        <v>1.25</v>
+      </c>
+      <c r="S522" s="31">
+        <v>0.78</v>
+      </c>
+      <c r="T522" s="31">
+        <v>0.66</v>
+      </c>
+      <c r="U522" s="31">
+        <v>0.67</v>
+      </c>
+      <c r="V522" s="31">
+        <v>1.17</v>
+      </c>
+      <c r="W522" s="31">
+        <v>1.33</v>
+      </c>
+      <c r="AC522" s="31">
+        <v>0.218</v>
+      </c>
+      <c r="AD522" s="31">
+        <v>0.126</v>
+      </c>
+      <c r="BE522" s="28">
+        <v>6.67</v>
+      </c>
+      <c r="BF522" s="30">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="523" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A523" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B523" s="26" t="s">
+        <v>743</v>
+      </c>
+      <c r="C523" s="27">
+        <v>38</v>
+      </c>
+      <c r="D523" s="27">
+        <v>38</v>
+      </c>
+      <c r="E523" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="I523" s="27">
+        <v>5.94</v>
+      </c>
+      <c r="K523" s="29">
+        <v>2.34</v>
+      </c>
+      <c r="L523" s="29">
+        <v>1.84</v>
+      </c>
+      <c r="M523" s="31">
+        <v>2.84</v>
+      </c>
+      <c r="N523" s="31">
+        <v>1.01</v>
+      </c>
+      <c r="O523" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P523" s="31">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Q523" s="31">
+        <v>2.11</v>
+      </c>
+      <c r="R523" s="31">
+        <v>1.38</v>
+      </c>
+      <c r="S523" s="31">
+        <v>0.72</v>
+      </c>
+      <c r="T523" s="31">
+        <v>0.77</v>
+      </c>
+      <c r="U523" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="V523" s="31">
+        <v>1.08</v>
+      </c>
+      <c r="W523" s="31">
+        <v>1.2</v>
+      </c>
+      <c r="AC523" s="31">
+        <v>0.08</v>
+      </c>
+      <c r="AD523" s="31">
+        <v>6.2E-2</v>
+      </c>
+      <c r="BE523" s="28">
+        <v>11.88</v>
+      </c>
+      <c r="BF523" s="30">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="524" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A524" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B524" s="26" t="s">
+        <v>744</v>
+      </c>
+      <c r="C524" s="27">
+        <v>38</v>
+      </c>
+      <c r="D524" s="27">
+        <v>38</v>
+      </c>
+      <c r="E524" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="I524" s="27">
+        <v>3.96</v>
+      </c>
+      <c r="K524" s="29">
+        <v>3.46</v>
+      </c>
+      <c r="L524" s="29">
+        <v>2.72</v>
+      </c>
+      <c r="M524" s="31">
+        <v>4.2</v>
+      </c>
+      <c r="N524" s="31">
+        <v>1.54</v>
+      </c>
+      <c r="O524" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P524" s="31">
+        <v>1.61</v>
+      </c>
+      <c r="Q524" s="31">
+        <v>3.02</v>
+      </c>
+      <c r="R524" s="31">
+        <v>2.08</v>
+      </c>
+      <c r="S524" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T524" s="31">
+        <v>0.78</v>
+      </c>
+      <c r="U524" s="31">
+        <v>0.93</v>
+      </c>
+      <c r="V524" s="31">
+        <v>1.65</v>
+      </c>
+      <c r="W524" s="31">
+        <v>1.85</v>
+      </c>
+      <c r="AC524" s="31">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="AD524" s="31">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="BE524" s="28">
+        <v>7.92</v>
+      </c>
+      <c r="BF524" s="30">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="525" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A525" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B525" s="26" t="s">
+        <v>745</v>
+      </c>
+      <c r="C525" s="27">
+        <v>38</v>
+      </c>
+      <c r="D525" s="27">
+        <v>38</v>
+      </c>
+      <c r="E525" s="27">
+        <v>6.4</v>
+      </c>
+      <c r="I525" s="27">
+        <v>2.97</v>
+      </c>
+      <c r="K525" s="29">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L525" s="29">
+        <v>3.57</v>
+      </c>
+      <c r="M525" s="31">
+        <v>5.37</v>
+      </c>
+      <c r="N525" s="31">
+        <v>2.02</v>
+      </c>
+      <c r="O525" s="31">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="P525" s="31">
+        <v>2.09</v>
+      </c>
+      <c r="Q525" s="31">
+        <v>3.99</v>
+      </c>
+      <c r="R525" s="31">
+        <v>2.64</v>
+      </c>
+      <c r="S525" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="T525" s="31">
+        <v>0.79</v>
+      </c>
+      <c r="U525" s="31">
+        <v>1.26</v>
+      </c>
+      <c r="V525" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="W525" s="31">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="AC525" s="31">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="AD525" s="31">
+        <v>0.499</v>
+      </c>
+      <c r="BE525" s="28">
+        <v>5.94</v>
+      </c>
+      <c r="BF525" s="30">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="526" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A526" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B526" s="26" t="s">
+        <v>746</v>
+      </c>
+      <c r="C526" s="27">
+        <v>45</v>
+      </c>
+      <c r="D526" s="27">
+        <v>45</v>
+      </c>
+      <c r="E526" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="I526" s="27">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="K526" s="29">
+        <v>4.13</v>
+      </c>
+      <c r="L526" s="29">
+        <v>3.24</v>
+      </c>
+      <c r="M526" s="31">
+        <v>7.07</v>
+      </c>
+      <c r="N526" s="31">
+        <v>2.16</v>
+      </c>
+      <c r="O526" s="31">
+        <v>1.31</v>
+      </c>
+      <c r="P526" s="31">
+        <v>2.29</v>
+      </c>
+      <c r="Q526" s="31">
+        <v>4.29</v>
+      </c>
+      <c r="R526" s="31">
+        <v>3.44</v>
+      </c>
+      <c r="S526" s="31">
+        <v>1.53</v>
+      </c>
+      <c r="T526" s="31">
+        <v>0.91</v>
+      </c>
+      <c r="U526" s="31">
+        <v>1.28</v>
+      </c>
+      <c r="V526" s="31">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W526" s="31">
+        <v>2.57</v>
+      </c>
+      <c r="AC526" s="31">
+        <v>0.314</v>
+      </c>
+      <c r="AD526" s="31">
+        <v>0.35</v>
+      </c>
+      <c r="BE526" s="28">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="BF526" s="30">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="527" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A527" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B527" s="26" t="s">
+        <v>747</v>
+      </c>
+      <c r="C527" s="27">
+        <v>51</v>
+      </c>
+      <c r="D527" s="27">
+        <v>51</v>
+      </c>
+      <c r="E527" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="I527" s="27">
+        <v>5.31</v>
+      </c>
+      <c r="K527" s="29">
+        <v>4.7</v>
+      </c>
+      <c r="L527" s="29">
+        <v>3.69</v>
+      </c>
+      <c r="M527" s="31">
+        <v>10.34</v>
+      </c>
+      <c r="N527" s="31">
+        <v>2.76</v>
+      </c>
+      <c r="O527" s="31">
+        <v>1.48</v>
+      </c>
+      <c r="P527" s="31">
+        <v>2.94</v>
+      </c>
+      <c r="Q527" s="31">
+        <v>5.53</v>
+      </c>
+      <c r="R527" s="31">
+        <v>4.99</v>
+      </c>
+      <c r="S527" s="31">
+        <v>1.96</v>
+      </c>
+      <c r="T527" s="31">
+        <v>1.03</v>
+      </c>
+      <c r="U527" s="31">
+        <v>1.64</v>
+      </c>
+      <c r="V527" s="31">
+        <v>2.94</v>
+      </c>
+      <c r="W527" s="31">
+        <v>3.27</v>
+      </c>
+      <c r="AC527" s="31">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="AD527" s="31">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="BE527" s="28">
+        <v>10.6</v>
+      </c>
+      <c r="BF527" s="30">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="528" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A528" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B528" s="26" t="s">
+        <v>748</v>
+      </c>
+      <c r="C528" s="27">
+        <v>51</v>
+      </c>
+      <c r="D528" s="27">
+        <v>51</v>
+      </c>
+      <c r="E528" s="27">
+        <v>6.4</v>
+      </c>
+      <c r="I528" s="27">
+        <v>3.98</v>
+      </c>
+      <c r="K528" s="29">
+        <v>6.2</v>
+      </c>
+      <c r="L528" s="29">
+        <v>4.87</v>
+      </c>
+      <c r="M528" s="31">
+        <v>13.52</v>
+      </c>
+      <c r="N528" s="31">
+        <v>3.69</v>
+      </c>
+      <c r="O528" s="31">
+        <v>1.48</v>
+      </c>
+      <c r="P528" s="31">
+        <v>3.88</v>
+      </c>
+      <c r="Q528" s="31">
+        <v>7.29</v>
+      </c>
+      <c r="R528" s="31">
+        <v>6.77</v>
+      </c>
+      <c r="S528" s="31">
+        <v>2.65</v>
+      </c>
+      <c r="T528" s="31">
+        <v>1.04</v>
+      </c>
+      <c r="U528" s="31">
+        <v>2.21</v>
+      </c>
+      <c r="V528" s="31">
+        <v>3.98</v>
+      </c>
+      <c r="W528" s="31">
+        <v>4.42</v>
+      </c>
+      <c r="AC528" s="31">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="AD528" s="31">
+        <v>1.2070000000000001</v>
+      </c>
+      <c r="BE528" s="28">
+        <v>7.97</v>
+      </c>
+      <c r="BF528" s="30">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="555" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>545</v>
+      </c>
+      <c r="B555" t="s">
+        <v>434</v>
+      </c>
+      <c r="C555" t="s">
+        <v>546</v>
+      </c>
+      <c r="D555" t="s">
+        <v>10</v>
+      </c>
+      <c r="E555" t="s">
+        <v>547</v>
+      </c>
+      <c r="F555" t="s">
+        <v>548</v>
+      </c>
+      <c r="G555" t="s">
+        <v>549</v>
+      </c>
+      <c r="H555" t="s">
+        <v>435</v>
+      </c>
+      <c r="I555" t="s">
+        <v>550</v>
+      </c>
+      <c r="J555" t="s">
+        <v>27</v>
+      </c>
+      <c r="K555" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="556" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>551</v>
+      </c>
+      <c r="B556" t="s">
+        <v>551</v>
+      </c>
+      <c r="C556" t="s">
+        <v>552</v>
+      </c>
+      <c r="D556" t="s">
+        <v>553</v>
+      </c>
+      <c r="E556" t="s">
+        <v>554</v>
+      </c>
+      <c r="F556" t="s">
+        <v>555</v>
+      </c>
+      <c r="G556" t="s">
+        <v>556</v>
+      </c>
+      <c r="H556" t="s">
+        <v>557</v>
+      </c>
+      <c r="I556" t="s">
+        <v>556</v>
+      </c>
+      <c r="J556" t="s">
+        <v>555</v>
+      </c>
+      <c r="K556" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="557" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A557">
+        <v>12.7</v>
+      </c>
+      <c r="B557">
+        <v>0.7</v>
+      </c>
+      <c r="C557">
+        <v>0.04</v>
+      </c>
+      <c r="D557">
+        <v>0.26</v>
+      </c>
+      <c r="E557">
+        <v>0.21</v>
+      </c>
+      <c r="F557">
+        <v>0.05</v>
+      </c>
+      <c r="G557">
+        <v>0.08</v>
+      </c>
+      <c r="H557">
+        <v>0.42</v>
+      </c>
+      <c r="I557">
+        <v>0.1</v>
+      </c>
+      <c r="J557">
+        <v>0.1</v>
+      </c>
+      <c r="K557">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="558" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A558">
+        <v>12.7</v>
+      </c>
+      <c r="B558">
+        <v>0.9</v>
+      </c>
+      <c r="C558">
+        <v>0.04</v>
+      </c>
+      <c r="D558">
+        <v>0.33</v>
+      </c>
+      <c r="E558">
+        <v>0.26</v>
+      </c>
+      <c r="F558">
+        <v>0.06</v>
+      </c>
+      <c r="G558">
+        <v>0.09</v>
+      </c>
+      <c r="H558">
+        <v>0.42</v>
+      </c>
+      <c r="I558">
+        <v>0.13</v>
+      </c>
+      <c r="J558">
+        <v>0.12</v>
+      </c>
+      <c r="K558">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="559" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A559">
+        <v>12.7</v>
+      </c>
+      <c r="B559">
+        <v>1.25</v>
+      </c>
+      <c r="C559">
+        <v>0.04</v>
+      </c>
+      <c r="D559">
+        <v>0.45</v>
+      </c>
+      <c r="E559">
+        <v>0.35</v>
+      </c>
+      <c r="F559">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G559">
+        <v>0.12</v>
+      </c>
+      <c r="H559">
+        <v>0.41</v>
+      </c>
+      <c r="I559">
+        <v>0.16</v>
+      </c>
+      <c r="J559">
+        <v>0.15</v>
+      </c>
+      <c r="K559">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="560" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A560">
+        <v>12.7</v>
+      </c>
+      <c r="B560">
+        <v>1.6</v>
+      </c>
+      <c r="C560">
+        <v>0.04</v>
+      </c>
+      <c r="D560">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E560">
+        <v>0.44</v>
+      </c>
+      <c r="F560">
+        <v>0.09</v>
+      </c>
+      <c r="G560">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H560">
+        <v>0.4</v>
+      </c>
+      <c r="I560">
+        <v>0.2</v>
+      </c>
+      <c r="J560">
+        <v>0.18</v>
+      </c>
+      <c r="K560">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="561" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A561">
+        <v>15.87</v>
+      </c>
+      <c r="B561">
+        <v>0.7</v>
+      </c>
+      <c r="C561">
+        <v>0.05</v>
+      </c>
+      <c r="D561">
+        <v>0.33</v>
+      </c>
+      <c r="E561">
+        <v>0.26</v>
+      </c>
+      <c r="F561">
+        <v>0.1</v>
+      </c>
+      <c r="G561">
+        <v>0.12</v>
+      </c>
+      <c r="H561">
+        <v>0.54</v>
+      </c>
+      <c r="I561">
+        <v>0.16</v>
+      </c>
+      <c r="J561">
+        <v>0.19</v>
+      </c>
+      <c r="K561">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="562" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A562">
+        <v>15.87</v>
+      </c>
+      <c r="B562">
+        <v>0.9</v>
+      </c>
+      <c r="C562">
+        <v>0.05</v>
+      </c>
+      <c r="D562">
+        <v>0.42</v>
+      </c>
+      <c r="E562">
+        <v>0.33</v>
+      </c>
+      <c r="F562">
+        <v>0.12</v>
+      </c>
+      <c r="G562">
+        <v>0.15</v>
+      </c>
+      <c r="H562">
+        <v>0.53</v>
+      </c>
+      <c r="I562">
+        <v>0.2</v>
+      </c>
+      <c r="J562">
+        <v>0.24</v>
+      </c>
+      <c r="K562">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="563" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A563">
+        <v>15.87</v>
+      </c>
+      <c r="B563">
+        <v>1.25</v>
+      </c>
+      <c r="C563">
+        <v>0.05</v>
+      </c>
+      <c r="D563">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E563">
+        <v>0.45</v>
+      </c>
+      <c r="F563">
+        <v>0.15</v>
+      </c>
+      <c r="G563">
+        <v>0.19</v>
+      </c>
+      <c r="H563">
+        <v>0.52</v>
+      </c>
+      <c r="I563">
+        <v>0.27</v>
+      </c>
+      <c r="J563">
+        <v>0.31</v>
+      </c>
+      <c r="K563">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="564" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A564">
+        <v>15.87</v>
+      </c>
+      <c r="B564">
+        <v>1.6</v>
+      </c>
+      <c r="C564">
+        <v>0.05</v>
+      </c>
+      <c r="D564">
+        <v>0.72</v>
+      </c>
+      <c r="E564">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F564">
+        <v>0.18</v>
+      </c>
+      <c r="G564">
+        <v>0.23</v>
+      </c>
+      <c r="H564">
+        <v>0.51</v>
+      </c>
+      <c r="I564">
+        <v>0.33</v>
+      </c>
+      <c r="J564">
+        <v>0.37</v>
+      </c>
+      <c r="K564">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="565" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A565">
+        <v>19.05</v>
+      </c>
+      <c r="B565">
+        <v>0.7</v>
+      </c>
+      <c r="C565">
+        <v>0.06</v>
+      </c>
+      <c r="D565">
+        <v>0.4</v>
+      </c>
+      <c r="E565">
+        <v>0.32</v>
+      </c>
+      <c r="F565">
+        <v>0.17</v>
+      </c>
+      <c r="G565">
+        <v>0.18</v>
+      </c>
+      <c r="H565">
+        <v>0.65</v>
+      </c>
+      <c r="I565">
+        <v>0.24</v>
+      </c>
+      <c r="J565">
+        <v>0.34</v>
+      </c>
+      <c r="K565">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="566" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A566">
+        <v>19.05</v>
+      </c>
+      <c r="B566">
+        <v>0.9</v>
+      </c>
+      <c r="C566">
+        <v>0.06</v>
+      </c>
+      <c r="D566">
+        <v>0.51</v>
+      </c>
+      <c r="E566">
+        <v>0.4</v>
+      </c>
+      <c r="F566">
+        <v>0.21</v>
+      </c>
+      <c r="G566">
+        <v>0.22</v>
+      </c>
+      <c r="H566">
+        <v>0.64</v>
+      </c>
+      <c r="I566">
+        <v>0.3</v>
+      </c>
+      <c r="J566">
+        <v>0.42</v>
+      </c>
+      <c r="K566">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="567" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A567">
+        <v>19.05</v>
+      </c>
+      <c r="B567">
+        <v>1.25</v>
+      </c>
+      <c r="C567">
+        <v>0.06</v>
+      </c>
+      <c r="D567">
+        <v>0.7</v>
+      </c>
+      <c r="E567">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F567">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G567">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H567">
+        <v>0.63</v>
+      </c>
+      <c r="I567">
+        <v>0.4</v>
+      </c>
+      <c r="J567">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K567">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="568" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A568">
+        <v>19.05</v>
+      </c>
+      <c r="B568">
+        <v>1.6</v>
+      </c>
+      <c r="C568">
+        <v>0.06</v>
+      </c>
+      <c r="D568">
+        <v>0.88</v>
+      </c>
+      <c r="E568">
+        <v>0.69</v>
+      </c>
+      <c r="F568">
+        <v>0.34</v>
+      </c>
+      <c r="G568">
+        <v>0.35</v>
+      </c>
+      <c r="H568">
+        <v>0.62</v>
+      </c>
+      <c r="I568">
+        <v>0.49</v>
+      </c>
+      <c r="J568">
+        <v>0.67</v>
+      </c>
+      <c r="K568">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="569" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A569">
+        <v>19.05</v>
+      </c>
+      <c r="B569">
+        <v>2</v>
+      </c>
+      <c r="C569">
+        <v>0.06</v>
+      </c>
+      <c r="D569">
+        <v>1.07</v>
+      </c>
+      <c r="E569">
+        <v>0.84</v>
+      </c>
+      <c r="F569">
+        <v>0.39</v>
+      </c>
+      <c r="G569">
+        <v>0.41</v>
+      </c>
+      <c r="H569">
+        <v>0.61</v>
+      </c>
+      <c r="I569">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J569">
+        <v>0.79</v>
+      </c>
+      <c r="K569">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="570" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A570">
+        <v>22.22</v>
+      </c>
+      <c r="B570">
+        <v>0.7</v>
+      </c>
+      <c r="C570">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D570">
+        <v>0.47</v>
+      </c>
+      <c r="E570">
+        <v>0.37</v>
+      </c>
+      <c r="F570">
+        <v>0.27</v>
+      </c>
+      <c r="G570">
+        <v>0.25</v>
+      </c>
+      <c r="H570">
+        <v>0.76</v>
+      </c>
+      <c r="I570">
+        <v>0.32</v>
+      </c>
+      <c r="J570">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K570">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="571" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A571">
+        <v>22.22</v>
+      </c>
+      <c r="B571">
+        <v>0.9</v>
+      </c>
+      <c r="C571">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D571">
+        <v>0.6</v>
+      </c>
+      <c r="E571">
+        <v>0.47</v>
+      </c>
+      <c r="F571">
+        <v>0.34</v>
+      </c>
+      <c r="G571">
+        <v>0.31</v>
+      </c>
+      <c r="H571">
+        <v>0.75</v>
+      </c>
+      <c r="I571">
+        <v>0.41</v>
+      </c>
+      <c r="J571">
+        <v>0.69</v>
+      </c>
+      <c r="K571">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="572" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A572">
+        <v>22.22</v>
+      </c>
+      <c r="B572">
+        <v>1.25</v>
+      </c>
+      <c r="C572">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D572">
+        <v>0.82</v>
+      </c>
+      <c r="E572">
+        <v>0.65</v>
+      </c>
+      <c r="F572">
+        <v>0.45</v>
+      </c>
+      <c r="G572">
+        <v>0.41</v>
+      </c>
+      <c r="H572">
+        <v>0.74</v>
+      </c>
+      <c r="I572">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J572">
+        <v>0.91</v>
+      </c>
+      <c r="K572">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="575" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>545</v>
+      </c>
+      <c r="B575" t="s">
+        <v>434</v>
+      </c>
+      <c r="C575" t="s">
+        <v>546</v>
+      </c>
+      <c r="D575" t="s">
+        <v>10</v>
+      </c>
+      <c r="E575" t="s">
+        <v>547</v>
+      </c>
+      <c r="F575" t="s">
+        <v>548</v>
+      </c>
+      <c r="G575" t="s">
+        <v>549</v>
+      </c>
+      <c r="H575" t="s">
+        <v>435</v>
+      </c>
+      <c r="I575" t="s">
+        <v>550</v>
+      </c>
+      <c r="J575" t="s">
+        <v>27</v>
+      </c>
+      <c r="K575" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="576" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>551</v>
+      </c>
+      <c r="B576" t="s">
+        <v>551</v>
+      </c>
+      <c r="C576" t="s">
+        <v>552</v>
+      </c>
+      <c r="D576" t="s">
+        <v>553</v>
+      </c>
+      <c r="E576" t="s">
+        <v>554</v>
+      </c>
+      <c r="F576" t="s">
+        <v>555</v>
+      </c>
+      <c r="G576" t="s">
+        <v>556</v>
+      </c>
+      <c r="H576" t="s">
+        <v>557</v>
+      </c>
+      <c r="I576" t="s">
+        <v>556</v>
+      </c>
+      <c r="J576" t="s">
+        <v>555</v>
+      </c>
+      <c r="K576" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="577" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>567</v>
+      </c>
+      <c r="B577" t="s">
+        <v>565</v>
+      </c>
+      <c r="C577" t="s">
+        <v>585</v>
+      </c>
+      <c r="D577" t="s">
+        <v>586</v>
+      </c>
+      <c r="E577" t="s">
+        <v>573</v>
+      </c>
+      <c r="F577" t="s">
+        <v>587</v>
+      </c>
+      <c r="G577" t="s">
+        <v>588</v>
+      </c>
+      <c r="H577" t="s">
+        <v>589</v>
+      </c>
+      <c r="I577" t="s">
+        <v>590</v>
+      </c>
+      <c r="J577" t="s">
+        <v>591</v>
+      </c>
+      <c r="K577" t="s">
+        <v>581</v>
+      </c>
+      <c r="L577" t="s">
+        <v>577</v>
+      </c>
+      <c r="M577" t="s">
+        <v>565</v>
+      </c>
+      <c r="N577" t="s">
+        <v>592</v>
+      </c>
+      <c r="O577" t="s">
+        <v>591</v>
+      </c>
+      <c r="P577" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q577" t="s">
+        <v>594</v>
+      </c>
+      <c r="R577" t="s">
+        <v>571</v>
+      </c>
+      <c r="S577" t="s">
+        <v>582</v>
+      </c>
+      <c r="T577" t="s">
+        <v>595</v>
+      </c>
+      <c r="U577" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="578" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>558</v>
+      </c>
+      <c r="B578" t="s">
+        <v>559</v>
+      </c>
+      <c r="C578" t="s">
+        <v>569</v>
+      </c>
+      <c r="D578" t="s">
+        <v>597</v>
+      </c>
+      <c r="E578" t="s">
+        <v>566</v>
+      </c>
+      <c r="F578" t="s">
+        <v>562</v>
+      </c>
+      <c r="G578" t="s">
+        <v>598</v>
+      </c>
+      <c r="H578" t="s">
+        <v>597</v>
+      </c>
+      <c r="I578" t="s">
+        <v>580</v>
+      </c>
+      <c r="J578" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="579" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>561</v>
+      </c>
+      <c r="B579" t="s">
+        <v>559</v>
+      </c>
+      <c r="C579" t="s">
+        <v>575</v>
+      </c>
+      <c r="D579" t="s">
+        <v>569</v>
+      </c>
+      <c r="E579" t="s">
+        <v>570</v>
+      </c>
+      <c r="F579" t="s">
+        <v>566</v>
+      </c>
+      <c r="G579" t="s">
+        <v>598</v>
+      </c>
+      <c r="H579" t="s">
+        <v>569</v>
+      </c>
+      <c r="I579" t="s">
+        <v>585</v>
+      </c>
+      <c r="J579" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="580" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>564</v>
+      </c>
+      <c r="B580" t="s">
+        <v>559</v>
+      </c>
+      <c r="C580" t="s">
+        <v>600</v>
+      </c>
+      <c r="D580" t="s">
+        <v>583</v>
+      </c>
+      <c r="E580" t="s">
+        <v>575</v>
+      </c>
+      <c r="F580" t="s">
+        <v>573</v>
+      </c>
+      <c r="G580" t="s">
+        <v>599</v>
+      </c>
+      <c r="H580" t="s">
+        <v>588</v>
+      </c>
+      <c r="I580" t="s">
+        <v>601</v>
+      </c>
+      <c r="J580" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="581" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>567</v>
+      </c>
+      <c r="B581" t="s">
+        <v>559</v>
+      </c>
+      <c r="C581" t="s">
+        <v>603</v>
+      </c>
+      <c r="D581" t="s">
+        <v>604</v>
+      </c>
+      <c r="E581" t="s">
+        <v>599</v>
+      </c>
+      <c r="F581" t="s">
+        <v>576</v>
+      </c>
+      <c r="G581" t="s">
+        <v>579</v>
+      </c>
+      <c r="H581" t="s">
+        <v>584</v>
+      </c>
+      <c r="I581" t="s">
+        <v>605</v>
+      </c>
+      <c r="J581" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="582" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>577</v>
+      </c>
+      <c r="B582" t="s">
+        <v>559</v>
+      </c>
+      <c r="C582" t="s">
+        <v>607</v>
+      </c>
+      <c r="D582" t="s">
+        <v>608</v>
+      </c>
+      <c r="E582" t="s">
+        <v>609</v>
+      </c>
+      <c r="F582" t="s">
+        <v>610</v>
+      </c>
+      <c r="G582" t="s">
+        <v>580</v>
+      </c>
+      <c r="H582" t="s">
+        <v>611</v>
+      </c>
+      <c r="I582" t="s">
+        <v>612</v>
+      </c>
+      <c r="J582" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="583" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="584" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>614</v>
+      </c>
+      <c r="B584" t="s">
+        <v>559</v>
+      </c>
+      <c r="C584" t="s">
+        <v>615</v>
+      </c>
+      <c r="D584" t="s">
+        <v>616</v>
+      </c>
+      <c r="E584" t="s">
+        <v>617</v>
+      </c>
+      <c r="F584" t="s">
+        <v>604</v>
+      </c>
+      <c r="G584" t="s">
+        <v>586</v>
+      </c>
+      <c r="H584" t="s">
+        <v>618</v>
+      </c>
+      <c r="I584" t="s">
+        <v>619</v>
+      </c>
+      <c r="J584" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="585" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>561</v>
+      </c>
+      <c r="B585" t="s">
+        <v>560</v>
+      </c>
+      <c r="C585" t="s">
+        <v>598</v>
+      </c>
+      <c r="D585" t="s">
+        <v>589</v>
+      </c>
+      <c r="E585" t="s">
+        <v>585</v>
+      </c>
+      <c r="F585" t="s">
+        <v>572</v>
+      </c>
+      <c r="G585" t="s">
+        <v>621</v>
+      </c>
+      <c r="H585" t="s">
+        <v>622</v>
+      </c>
+      <c r="I585" t="s">
+        <v>623</v>
+      </c>
+      <c r="J585" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="586" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>564</v>
+      </c>
+      <c r="B586" t="s">
+        <v>560</v>
+      </c>
+      <c r="C586" t="s">
+        <v>603</v>
+      </c>
+      <c r="D586" t="s">
+        <v>604</v>
+      </c>
+      <c r="E586" t="s">
+        <v>624</v>
+      </c>
+      <c r="F586" t="s">
+        <v>574</v>
+      </c>
+      <c r="G586" t="s">
+        <v>625</v>
+      </c>
+      <c r="H586" t="s">
+        <v>626</v>
+      </c>
+      <c r="I586" t="s">
+        <v>627</v>
+      </c>
+      <c r="J586" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="587" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>567</v>
+      </c>
+      <c r="B587" t="s">
+        <v>560</v>
+      </c>
+      <c r="C587" t="s">
+        <v>629</v>
+      </c>
+      <c r="D587" t="s">
+        <v>617</v>
+      </c>
+      <c r="E587" t="s">
+        <v>630</v>
+      </c>
+      <c r="F587" t="s">
+        <v>621</v>
+      </c>
+      <c r="G587" t="s">
+        <v>578</v>
+      </c>
+      <c r="H587" t="s">
+        <v>631</v>
+      </c>
+      <c r="I587" t="s">
+        <v>632</v>
+      </c>
+      <c r="J587" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="588" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>577</v>
+      </c>
+      <c r="B588" t="s">
+        <v>560</v>
+      </c>
+      <c r="C588" t="s">
+        <v>634</v>
+      </c>
+      <c r="D588" t="s">
+        <v>607</v>
+      </c>
+      <c r="E588" t="s">
+        <v>623</v>
+      </c>
+      <c r="F588" t="s">
+        <v>595</v>
+      </c>
+      <c r="G588" t="s">
+        <v>635</v>
+      </c>
+      <c r="H588" t="s">
+        <v>636</v>
+      </c>
+      <c r="I588" t="s">
+        <v>637</v>
+      </c>
+      <c r="J588" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="589" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>614</v>
+      </c>
+      <c r="B589" t="s">
+        <v>560</v>
+      </c>
+      <c r="C589" t="s">
+        <v>639</v>
+      </c>
+      <c r="D589" t="s">
+        <v>615</v>
+      </c>
+      <c r="E589" t="s">
+        <v>640</v>
+      </c>
+      <c r="F589" t="s">
+        <v>641</v>
+      </c>
+      <c r="G589" t="s">
+        <v>585</v>
+      </c>
+      <c r="H589" t="s">
+        <v>642</v>
+      </c>
+      <c r="I589" t="s">
+        <v>643</v>
+      </c>
+      <c r="J589" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="590" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="591" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>646</v>
+      </c>
+      <c r="B591" t="s">
+        <v>560</v>
+      </c>
+      <c r="C591" t="s">
+        <v>647</v>
+      </c>
+      <c r="D591" t="s">
+        <v>648</v>
+      </c>
+      <c r="E591" t="s">
+        <v>649</v>
+      </c>
+      <c r="F591" t="s">
+        <v>634</v>
+      </c>
+      <c r="G591" t="s">
+        <v>650</v>
+      </c>
+      <c r="H591" t="s">
+        <v>638</v>
+      </c>
+      <c r="I591" t="s">
+        <v>651</v>
+      </c>
+      <c r="J591" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="592" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>561</v>
+      </c>
+      <c r="B592" t="s">
+        <v>563</v>
+      </c>
+      <c r="C592" t="s">
+        <v>635</v>
+      </c>
+      <c r="D592" t="s">
+        <v>580</v>
+      </c>
+      <c r="E592" t="s">
+        <v>653</v>
+      </c>
+      <c r="F592" t="s">
+        <v>654</v>
+      </c>
+      <c r="G592" t="s">
+        <v>618</v>
+      </c>
+      <c r="H592" t="s">
+        <v>564</v>
+      </c>
+      <c r="I592" t="s">
+        <v>655</v>
+      </c>
+      <c r="J592" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="593" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>564</v>
+      </c>
+      <c r="B593" t="s">
+        <v>563</v>
+      </c>
+      <c r="C593" t="s">
+        <v>657</v>
+      </c>
+      <c r="D593" t="s">
+        <v>602</v>
+      </c>
+      <c r="E593" t="s">
+        <v>658</v>
+      </c>
+      <c r="F593" t="s">
+        <v>659</v>
+      </c>
+      <c r="G593" t="s">
+        <v>660</v>
+      </c>
+      <c r="H593" t="s">
+        <v>605</v>
+      </c>
+      <c r="I593" t="s">
+        <v>661</v>
+      </c>
+      <c r="J593" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>567</v>
+      </c>
+      <c r="B594" t="s">
+        <v>563</v>
+      </c>
+      <c r="C594" t="s">
+        <v>628</v>
+      </c>
+      <c r="D594" t="s">
+        <v>663</v>
+      </c>
+      <c r="E594" t="s">
+        <v>664</v>
+      </c>
+      <c r="F594" t="s">
+        <v>665</v>
+      </c>
+      <c r="G594" t="s">
+        <v>659</v>
+      </c>
+      <c r="H594" t="s">
+        <v>666</v>
+      </c>
+      <c r="I594" t="s">
+        <v>667</v>
+      </c>
+      <c r="J594" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>577</v>
+      </c>
+      <c r="B595" t="s">
+        <v>563</v>
+      </c>
+      <c r="C595" t="s">
+        <v>669</v>
+      </c>
+      <c r="D595" t="s">
+        <v>670</v>
+      </c>
+      <c r="E595" t="s">
+        <v>671</v>
+      </c>
+      <c r="F595" t="s">
+        <v>672</v>
+      </c>
+      <c r="G595" t="s">
+        <v>673</v>
+      </c>
+      <c r="H595" t="s">
+        <v>674</v>
+      </c>
+      <c r="I595" t="s">
+        <v>675</v>
+      </c>
+      <c r="J595" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>614</v>
+      </c>
+      <c r="B596" t="s">
+        <v>563</v>
+      </c>
+      <c r="C596" t="s">
+        <v>677</v>
+      </c>
+      <c r="D596" t="s">
+        <v>678</v>
+      </c>
+      <c r="E596" t="s">
+        <v>679</v>
+      </c>
+      <c r="F596" t="s">
+        <v>680</v>
+      </c>
+      <c r="G596" t="s">
+        <v>681</v>
+      </c>
+      <c r="H596" t="s">
+        <v>682</v>
+      </c>
+      <c r="I596" t="s">
+        <v>683</v>
+      </c>
+      <c r="J596" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>646</v>
+      </c>
+      <c r="B598" t="s">
+        <v>563</v>
+      </c>
+      <c r="C598" t="s">
+        <v>686</v>
+      </c>
+      <c r="D598" t="s">
+        <v>687</v>
+      </c>
+      <c r="E598" t="s">
+        <v>688</v>
+      </c>
+      <c r="F598" t="s">
+        <v>689</v>
+      </c>
+      <c r="G598" t="s">
+        <v>690</v>
+      </c>
+      <c r="H598" t="s">
+        <v>691</v>
+      </c>
+      <c r="I598" t="s">
+        <v>692</v>
+      </c>
+      <c r="J598" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="599" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>561</v>
+      </c>
+      <c r="B599" t="s">
+        <v>568</v>
+      </c>
+      <c r="C599" t="s">
+        <v>694</v>
+      </c>
+      <c r="D599" t="s">
+        <v>695</v>
+      </c>
+      <c r="E599" t="s">
+        <v>696</v>
+      </c>
+      <c r="F599" t="s">
+        <v>595</v>
+      </c>
+      <c r="G599" t="s">
+        <v>697</v>
+      </c>
+      <c r="H599" t="s">
+        <v>698</v>
+      </c>
+      <c r="I599" t="s">
+        <v>699</v>
+      </c>
+      <c r="J599" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="600" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>564</v>
+      </c>
+      <c r="B600" t="s">
+        <v>568</v>
+      </c>
+      <c r="C600" t="s">
+        <v>605</v>
+      </c>
+      <c r="D600" t="s">
+        <v>701</v>
+      </c>
+      <c r="E600" t="s">
+        <v>702</v>
+      </c>
+      <c r="F600" t="s">
+        <v>670</v>
+      </c>
+      <c r="G600" t="s">
+        <v>703</v>
+      </c>
+      <c r="H600" t="s">
+        <v>704</v>
+      </c>
+      <c r="I600" t="s">
+        <v>705</v>
+      </c>
+      <c r="J600" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="601" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>567</v>
+      </c>
+      <c r="B601" t="s">
+        <v>568</v>
+      </c>
+      <c r="C601" t="s">
+        <v>707</v>
+      </c>
+      <c r="D601" t="s">
+        <v>708</v>
+      </c>
+      <c r="E601" t="s">
+        <v>643</v>
+      </c>
+      <c r="F601" t="s">
+        <v>709</v>
+      </c>
+      <c r="G601" t="s">
+        <v>629</v>
+      </c>
+      <c r="H601" t="s">
+        <v>710</v>
+      </c>
+      <c r="I601" t="s">
+        <v>711</v>
+      </c>
+      <c r="J601" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="602" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>577</v>
+      </c>
+      <c r="B602" t="s">
+        <v>568</v>
+      </c>
+      <c r="C602" t="s">
+        <v>713</v>
+      </c>
+      <c r="D602" t="s">
+        <v>714</v>
+      </c>
+      <c r="E602" t="s">
+        <v>715</v>
+      </c>
+      <c r="F602" t="s">
+        <v>716</v>
+      </c>
+      <c r="G602" t="s">
+        <v>717</v>
+      </c>
+      <c r="H602" t="s">
+        <v>718</v>
+      </c>
+      <c r="I602" t="s">
+        <v>719</v>
+      </c>
+      <c r="J602" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="603" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>614</v>
+      </c>
+      <c r="B603" t="s">
+        <v>568</v>
+      </c>
+      <c r="C603" t="s">
+        <v>720</v>
+      </c>
+      <c r="D603" t="s">
+        <v>721</v>
+      </c>
+      <c r="E603" t="s">
+        <v>722</v>
+      </c>
+      <c r="F603" t="s">
+        <v>723</v>
+      </c>
+      <c r="G603" t="s">
+        <v>724</v>
+      </c>
+      <c r="H603" t="s">
+        <v>725</v>
+      </c>
+      <c r="I603" t="s">
+        <v>726</v>
+      </c>
+      <c r="J603" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="604" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="605" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>646</v>
+      </c>
+      <c r="B605" t="s">
+        <v>568</v>
+      </c>
+      <c r="C605" t="s">
+        <v>637</v>
+      </c>
+      <c r="D605" t="s">
+        <v>729</v>
+      </c>
+      <c r="E605" t="s">
+        <v>730</v>
+      </c>
+      <c r="F605" t="s">
+        <v>731</v>
+      </c>
+      <c r="G605" t="s">
+        <v>631</v>
+      </c>
+      <c r="H605" t="s">
+        <v>732</v>
+      </c>
+      <c r="I605" t="s">
+        <v>733</v>
+      </c>
+      <c r="J605" t="s">
+        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>